<commit_message>
Alteração nas colunas da planilha
</commit_message>
<xml_diff>
--- a/web-scraping/atualizar-indicadores/Investimento.xlsx
+++ b/web-scraping/atualizar-indicadores/Investimento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmnso\Documents\GitHub\python\web-scraping\atualizar-indicadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18788BB5-5812-4091-AE46-C591320BB1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D55FB8-6156-4101-812A-4ADF76D378ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28785" yWindow="7920" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Preço</t>
   </si>
@@ -321,7 +321,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -359,23 +359,14 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -887,14 +878,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.77734375" style="1" customWidth="1"/>
-    <col min="7" max="23" width="14.21875" style="1" hidden="1"/>
+    <col min="7" max="23" width="14.21875" style="1" hidden="1" customWidth="1"/>
     <col min="24" max="16384" width="8.88671875" style="1" hidden="1"/>
   </cols>
   <sheetData>
@@ -907,9 +899,6 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -920,8 +909,7 @@
       <c r="C3" s="12">
         <v>57.15</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14">
+      <c r="D3" s="13">
         <v>8.8699999999999987E-2</v>
       </c>
     </row>
@@ -929,11 +917,10 @@
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>54.77</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="9">
+      <c r="D4" s="9">
         <v>0.1205</v>
       </c>
     </row>
@@ -941,11 +928,10 @@
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>32.729999999999997</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="9">
+      <c r="D5" s="9">
         <v>0</v>
       </c>
     </row>
@@ -953,11 +939,10 @@
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>100.62</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="9">
+      <c r="D6" s="9">
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
@@ -965,19 +950,18 @@
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="15">
         <v>50.6</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="10">
+      <c r="D7" s="10">
         <v>5.3099999999999987E-2</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="2:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -997,10 +981,10 @@
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>8.4</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>9.89</v>
       </c>
       <c r="E10" s="9">
@@ -1011,10 +995,10 @@
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>99.8</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>104.21</v>
       </c>
       <c r="E11" s="9">
@@ -1025,10 +1009,10 @@
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>122.66</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>127.75</v>
       </c>
       <c r="E12" s="9">
@@ -1039,10 +1023,10 @@
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>103.79</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>101.82</v>
       </c>
       <c r="E13" s="9">
@@ -1053,10 +1037,10 @@
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>9.51</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>9.48</v>
       </c>
       <c r="E14" s="9">
@@ -1067,10 +1051,10 @@
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>99.88</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>103.88</v>
       </c>
       <c r="E15" s="9">
@@ -1081,10 +1065,10 @@
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>7.65</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>8.57</v>
       </c>
       <c r="E16" s="9">
@@ -1095,10 +1079,10 @@
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>103.06</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>123.95</v>
       </c>
       <c r="E17" s="9">
@@ -1109,10 +1093,10 @@
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>98</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>106.9</v>
       </c>
       <c r="E18" s="9">
@@ -1123,10 +1107,10 @@
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="15">
         <v>100.52</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="15">
         <v>117.39</v>
       </c>
       <c r="E19" s="10">
@@ -1134,76 +1118,76 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="18"/>
     </row>
     <row r="29" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
     </row>
     <row r="30" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="2:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="3:7" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>